<commit_message>
fix xslx et plots
</commit_message>
<xml_diff>
--- a/results/current_run/percentages.xlsx
+++ b/results/current_run/percentages.xlsx
@@ -452,7 +452,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>100</v>
+        <v>90</v>
       </c>
     </row>
     <row r="3">
@@ -532,7 +532,7 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>